<commit_message>
Se termina la app
</commit_message>
<xml_diff>
--- a/src/test/java/Hexaware/data/datacucumber.xlsx
+++ b/src/test/java/Hexaware/data/datacucumber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\netza\eclipse-workspace\ParaBank\src\test\java\Hexaware\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053E87D7-D7E5-4202-A13F-12A55189D526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A2730A-ACA2-438B-8901-81EAFAF62457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{29119E3F-C133-4130-A567-DA82EBA1B1E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>firstName</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Virginia</t>
   </si>
   <si>
-    <t>nlimas</t>
-  </si>
-  <si>
     <t>Olga</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>Texas</t>
-  </si>
-  <si>
-    <t>ocanchola</t>
   </si>
   <si>
     <t>username</t>
@@ -169,7 +163,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -468,10 +462,10 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
@@ -522,13 +516,13 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
         <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -556,8 +550,9 @@
       <c r="H2">
         <v>123123123</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
+      <c r="I2" t="str">
+        <f ca="1">_xlfn.CONCAT("nlimas",RANDBETWEEN(1,100))</f>
+        <v>nlimas23</v>
       </c>
       <c r="J2">
         <v>123123</v>
@@ -565,31 +560,33 @@
       <c r="K2">
         <v>123123</v>
       </c>
-      <c r="L2" t="s">
-        <v>15</v>
+      <c r="L2" t="str">
+        <f ca="1">I2</f>
+        <v>nlimas23</v>
       </c>
       <c r="M2">
+        <f>K2</f>
         <v>123123</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3">
         <v>122121</v>
@@ -600,8 +597,9 @@
       <c r="H3">
         <v>929929292</v>
       </c>
-      <c r="I3" t="s">
-        <v>21</v>
+      <c r="I3" t="str">
+        <f ca="1">_xlfn.CONCAT("ocanchola",RANDBETWEEN(1,100))</f>
+        <v>ocanchola56</v>
       </c>
       <c r="J3">
         <v>432323</v>
@@ -609,14 +607,16 @@
       <c r="K3">
         <v>432323</v>
       </c>
-      <c r="L3" t="s">
-        <v>21</v>
+      <c r="L3" t="str">
+        <f ca="1">I3</f>
+        <v>ocanchola56</v>
       </c>
       <c r="M3">
+        <f>K3</f>
         <v>432323</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>